<commit_message>
finally done! sorry for the messy code
</commit_message>
<xml_diff>
--- a/Tang_overall_metrics.xlsx
+++ b/Tang_overall_metrics.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7537058152793614</v>
+        <v>0.5017037157228622</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7537058152793614</v>
+        <v>0.5017037157228622</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7020711630377058</v>
+        <v>0.5451339915373766</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02321955435759562</v>
+        <v>0.148407217410269</v>
       </c>
       <c r="F2" t="n">
-        <v>2.505805590216966</v>
+        <v>3.382615389267453</v>
       </c>
       <c r="G2" t="n">
-        <v>877</v>
+        <v>6163</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5177956371986223</v>
+        <v>0.6510359869138496</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5177956371986223</v>
+        <v>0.6510359869138496</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5404433792690234</v>
+        <v>0.5931445603576752</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03284392543146995</v>
+        <v>0.06505041191066246</v>
       </c>
       <c r="F3" t="n">
-        <v>3.568863924840461</v>
+        <v>3.321614489972583</v>
       </c>
       <c r="G3" t="n">
-        <v>871</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2609970674486803</v>
+        <v>0.630192878338279</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2609970674486803</v>
+        <v>0.630192878338279</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3242258652094718</v>
+        <v>0.5702777544684065</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01667557427864234</v>
+        <v>0.1345874138558461</v>
       </c>
       <c r="F4" t="n">
-        <v>4.628278744949636</v>
+        <v>3.506261720912169</v>
       </c>
       <c r="G4" t="n">
-        <v>341</v>
+        <v>5392</v>
       </c>
     </row>
     <row r="5">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6467153284671533</v>
+        <v>0.3377982419422352</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6467153284671533</v>
+        <v>0.3377982419422352</v>
       </c>
       <c r="D5" t="n">
-        <v>0.654357459379616</v>
+        <v>0.3779859484777517</v>
       </c>
       <c r="E5" t="n">
-        <v>0.07990381864246314</v>
+        <v>0.07477551683647496</v>
       </c>
       <c r="F5" t="n">
-        <v>2.760006208612146</v>
+        <v>4.396762830076731</v>
       </c>
       <c r="G5" t="n">
-        <v>2740</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="6">
@@ -577,22 +577,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6636942675159235</v>
+        <v>0.5311121999020089</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6636942675159235</v>
+        <v>0.5311121999020089</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6760088231477878</v>
+        <v>0.4716119208179247</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1041466389181126</v>
+        <v>0.06218648568681087</v>
       </c>
       <c r="F6" t="n">
-        <v>2.511300507965821</v>
+        <v>4.279990209406025</v>
       </c>
       <c r="G6" t="n">
-        <v>3925</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="7">
@@ -602,22 +602,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8196581196581196</v>
+        <v>0.4044054747647562</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8196581196581196</v>
+        <v>0.4044054747647562</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8034068695895001</v>
+        <v>0.4368718955758346</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1214032428766383</v>
+        <v>0.1375679557111161</v>
       </c>
       <c r="F7" t="n">
-        <v>1.636764746270165</v>
+        <v>4.132687312799809</v>
       </c>
       <c r="G7" t="n">
-        <v>7020</v>
+        <v>4676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>